<commit_message>
Data through 6th Ipam
</commit_message>
<xml_diff>
--- a/ACervStresstestSchedule.xlsx
+++ b/ACervStresstestSchedule.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
   <si>
     <t>Wednesday</t>
   </si>
@@ -209,6 +209,21 @@
   </si>
   <si>
     <t xml:space="preserve">Yes in separate tanks and clean bases </t>
+  </si>
+  <si>
+    <t>30-32</t>
+  </si>
+  <si>
+    <t>87 @ 15:30</t>
+  </si>
+  <si>
+    <t>Switch 5 micron to 20 micron</t>
+  </si>
+  <si>
+    <t>Remove 1 micron filter @ 12:30</t>
+  </si>
+  <si>
+    <t>Y @ 12:30 set to 87</t>
   </si>
 </sst>
 </file>
@@ -696,11 +711,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1375325568"/>
-        <c:axId val="-1375321200"/>
+        <c:axId val="-225836464"/>
+        <c:axId val="-260207696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1375325568"/>
+        <c:axId val="-225836464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,7 +813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1375321200"/>
+        <c:crossAx val="-260207696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -806,7 +821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1375321200"/>
+        <c:axId val="-260207696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,7 +935,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1375325568"/>
+        <c:crossAx val="-225836464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1810,8 +1825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2436,23 +2451,27 @@
       <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="E19" s="3">
         <v>88.6</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="4" t="e">
         <f t="shared" si="2"/>
-        <v>31.111111111111111</v>
-      </c>
-      <c r="G19" s="3">
-        <v>88</v>
-      </c>
-      <c r="H19" s="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="M19" s="3"/>
     </row>
@@ -2466,24 +2485,30 @@
       <c r="C20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="E20" s="5">
         <v>88.6</v>
       </c>
       <c r="F20" s="6">
         <f t="shared" si="2"/>
-        <v>31.111111111111111</v>
+        <v>30.555555555555557</v>
       </c>
       <c r="G20" s="5">
-        <v>88</v>
-      </c>
-      <c r="H20" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5">
         <v>6</v>
       </c>
       <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+      <c r="L20" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Data processing through June 9 afternoon
</commit_message>
<xml_diff>
--- a/ACervStresstestSchedule.xlsx
+++ b/ACervStresstestSchedule.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="70">
   <si>
     <t>Wednesday</t>
   </si>
@@ -224,6 +224,21 @@
   </si>
   <si>
     <t>Y @ 12:30 set to 87</t>
+  </si>
+  <si>
+    <t>31-32</t>
+  </si>
+  <si>
+    <t>Switched 20 micron to 5 micron @ 13:00</t>
+  </si>
+  <si>
+    <t>Yes @ 13:30</t>
+  </si>
+  <si>
+    <t>Yes T2. 18 genotypes w/ fragments &gt;= 8</t>
+  </si>
+  <si>
+    <t>88@ 16:00</t>
   </si>
 </sst>
 </file>
@@ -711,11 +726,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-225836464"/>
-        <c:axId val="-260207696"/>
+        <c:axId val="-1466832352"/>
+        <c:axId val="-1465590320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-225836464"/>
+        <c:axId val="-1466832352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +828,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-260207696"/>
+        <c:crossAx val="-1465590320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -821,7 +836,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-260207696"/>
+        <c:axId val="-1465590320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -935,7 +950,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-225836464"/>
+        <c:crossAx val="-1466832352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1826,7 +1841,7 @@
   <dimension ref="A2:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2521,23 +2536,31 @@
       <c r="C21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="E21" s="3">
         <v>89.6</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="4" t="e">
         <f t="shared" si="2"/>
-        <v>31.666666666666668</v>
-      </c>
-      <c r="G21" s="3">
-        <v>89</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
+      <c r="K21" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="L21" s="3" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="M21" s="3"/>
     </row>

</xml_diff>

<commit_message>
Data through 8th Ipam w/ temperature through June 11
</commit_message>
<xml_diff>
--- a/ACervStresstestSchedule.xlsx
+++ b/ACervStresstestSchedule.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
   <si>
     <t>Wednesday</t>
   </si>
@@ -112,9 +112,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>For Chart</t>
-  </si>
-  <si>
     <t>Projected Temperature (oC)</t>
   </si>
   <si>
@@ -239,6 +236,54 @@
   </si>
   <si>
     <t>88@ 16:00</t>
+  </si>
+  <si>
+    <t>89 @ 15:00</t>
+  </si>
+  <si>
+    <t>32-33</t>
+  </si>
+  <si>
+    <t>31.5-32.5</t>
+  </si>
+  <si>
+    <t>Y to 88</t>
+  </si>
+  <si>
+    <t>Y Set to 88</t>
+  </si>
+  <si>
+    <t>Set to 88</t>
+  </si>
+  <si>
+    <t>Switch 5 microns</t>
+  </si>
+  <si>
+    <t>Days Seeing 32</t>
+  </si>
+  <si>
+    <t>88@ 16:30</t>
+  </si>
+  <si>
+    <t>5 microns switch @ 21:15</t>
+  </si>
+  <si>
+    <t>5 microns @ 9:00</t>
+  </si>
+  <si>
+    <t>89 @ 13:00</t>
+  </si>
+  <si>
+    <t>Set to 89</t>
+  </si>
+  <si>
+    <t>Yes @ 1200</t>
+  </si>
+  <si>
+    <t>Y. 2 @ 90. @ 13:00</t>
+  </si>
+  <si>
+    <t>H 88 Chill 89 @13:00</t>
   </si>
 </sst>
 </file>
@@ -268,7 +313,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,8 +338,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -317,13 +368,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -345,14 +406,87 @@
     <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -482,70 +616,25 @@
               <c:strCache>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>Monday</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>Tuesday</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Initial iPAM</c:v>
+                  <c:v>Wednesday</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Initial Sample</c:v>
+                  <c:v>Thursday</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.55555556</c:v>
+                  <c:v>Friday</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>iPAM</c:v>
+                  <c:v>Saturday</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.11111111</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>28.11111111</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28.66666667</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>iPAM</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>29.22222222</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>29.22222222</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>iPAM</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>29.77777778</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30.33333333</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>30.33333333</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>iPAM</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>30.88888889</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>31.44444444</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>iPAM</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>32</c:v>
+                  <c:v>Sunday</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -572,70 +661,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>-9.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>18.0</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -644,73 +688,28 @@
             <c:numRef>
               <c:f>Sheet1!$B$31:$B$52</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>27.0</c:v>
+                  <c:v>42905.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.0</c:v>
+                  <c:v>42906.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.0</c:v>
+                  <c:v>42907.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>42908.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.55555555555555</c:v>
+                  <c:v>42909.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.55555555555555</c:v>
+                  <c:v>42910.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.11111111111111</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>28.11111111111111</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28.66666666666667</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>28.66666666666667</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>29.22222222222222</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>29.22222222222222</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>29.77777777777778</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>29.77777777777778</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30.33333333333333</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>30.33333333333333</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>30.88888888888889</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>30.88888888888889</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>31.44444444444444</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>31.44444444444444</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>32.0</c:v>
+                  <c:v>42911.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,11 +725,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1466832352"/>
-        <c:axId val="-1465590320"/>
+        <c:axId val="-873007120"/>
+        <c:axId val="-873003088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1466832352"/>
+        <c:axId val="-873007120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -828,7 +827,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465590320"/>
+        <c:crossAx val="-873003088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -836,7 +835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1465590320"/>
+        <c:axId val="-873003088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -950,7 +949,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1466832352"/>
+        <c:crossAx val="-873007120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1838,10 +1837,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M52"/>
+  <dimension ref="A2:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1858,1089 +1860,1231 @@
     <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="M2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>42877</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>27</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>80.599999999999994</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <f>(E3-32)*5/9</f>
         <v>26.999999999999996</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>42878</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>27</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <f>D4*(9/5)+32</f>
         <v>80.599999999999994</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <f t="shared" ref="F4:F6" si="0">(E4-32)*5/9</f>
         <v>26.999999999999996</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5" t="s">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>42879</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>81.599999999999994</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <f t="shared" si="0"/>
         <v>27.555555555555554</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="G5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>42880</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4">
         <v>81.599999999999994</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>27.555555555555554</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="G6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5">
+      <c r="I6" s="4"/>
+      <c r="J6" s="4">
         <v>2</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>42881</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="D7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="2">
         <v>82.6</v>
       </c>
-      <c r="F7" s="4" t="e">
+      <c r="F7" s="3" t="e">
         <f t="shared" ref="F7:F9" si="1">(G7-32)*5/9</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>42882</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="D8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="4">
         <v>82.6</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <f t="shared" si="1"/>
         <v>27.777777777777779</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>82</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>42883</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="2">
         <v>83.6</v>
       </c>
-      <c r="F9" s="4" t="e">
+      <c r="F9" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="G9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7">
+        <v>42884</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8">
-        <v>42884</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>83.6</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <f>(G10-32)*5/9</f>
         <v>28.333333333333332</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>83</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5">
+      <c r="I10" s="4"/>
+      <c r="J10" s="4">
         <v>3</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>42885</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>30</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>84.6</v>
       </c>
-      <c r="F11" s="4" t="e">
+      <c r="F11" s="3" t="e">
         <f t="shared" ref="F11:F26" si="2">(G11-32)*5/9</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="G11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <v>8</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>42886</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="5">
+      <c r="D12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="4">
         <v>84.6</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <f t="shared" si="2"/>
         <v>28.888888888888889</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>84</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5" t="s">
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5" t="s">
+      <c r="L12" s="4"/>
+      <c r="M12" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>42887</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="D13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="2">
         <v>85.6</v>
       </c>
-      <c r="F13" s="4" t="e">
+      <c r="F13" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="G13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
         <v>4</v>
       </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>10</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>42888</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="D14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="4">
         <v>85.6</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <f t="shared" si="2"/>
         <v>29.444444444444443</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>85</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="I14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="7">
-        <v>37775</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="6">
+        <v>42889</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="3">
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="2">
         <v>86.6</v>
       </c>
-      <c r="F15" s="4" t="e">
+      <c r="F15" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>42890</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="D16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="4">
         <v>86.6</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>86</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6">
+        <v>42891</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>13</v>
-      </c>
-      <c r="B17" s="7">
-        <v>42891</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>87.6</v>
       </c>
-      <c r="F17" s="4" t="e">
+      <c r="F17" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3">
+      <c r="H17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2">
         <v>5</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
         <v>14</v>
       </c>
       <c r="B18" s="7">
         <v>42892</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="5">
+      <c r="D18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="4">
         <v>87.6</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>86</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5" t="s">
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
+      <c r="B19" s="6">
+        <v>42893</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>15</v>
-      </c>
-      <c r="B19" s="8">
-        <v>42893</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>88.6</v>
       </c>
-      <c r="F19" s="4" t="e">
+      <c r="F19" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
         <v>16</v>
       </c>
       <c r="B20" s="7">
-        <v>37780</v>
-      </c>
-      <c r="C20" s="5" t="s">
+        <v>42894</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="5">
+      <c r="D20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="4">
         <v>88.6</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <f t="shared" si="2"/>
         <v>30.555555555555557</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>87</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4">
+        <v>6</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>17</v>
+      </c>
+      <c r="B21" s="6">
+        <v>42895</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5">
-        <v>6</v>
-      </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="M20" s="5"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>17</v>
-      </c>
-      <c r="B21" s="8">
-        <v>42895</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>89.6</v>
       </c>
-      <c r="F21" s="4" t="e">
+      <c r="F21" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3" t="s">
+      <c r="H21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M21" s="3"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
+      <c r="L21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
         <v>18</v>
       </c>
       <c r="B22" s="7">
         <v>42896</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5">
+      <c r="D22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="4">
         <v>89.6</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
+        <f t="shared" si="2"/>
+        <v>31.111111111111111</v>
+      </c>
+      <c r="G22" s="4">
+        <v>88</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>19</v>
+      </c>
+      <c r="B23" s="6">
+        <v>42897</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="2">
+        <v>90.6</v>
+      </c>
+      <c r="F23" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>20</v>
+      </c>
+      <c r="B24" s="7">
+        <v>42898</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="4">
+        <v>33</v>
+      </c>
+      <c r="E24" s="4">
+        <v>90.6</v>
+      </c>
+      <c r="F24" s="5" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4">
+        <v>7</v>
+      </c>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>21</v>
+      </c>
+      <c r="B25" s="6">
+        <v>42899</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2">
+        <v>91.6</v>
+      </c>
+      <c r="F25" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>22</v>
+      </c>
+      <c r="B26" s="7">
+        <v>42900</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="4">
+        <v>91.6</v>
+      </c>
+      <c r="F26" s="5">
         <f t="shared" si="2"/>
         <v>31.666666666666668</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G26" s="4">
         <v>89</v>
       </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <v>19</v>
-      </c>
-      <c r="B23" s="7">
-        <v>42897</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="H26" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>23</v>
+      </c>
+      <c r="B27" s="6">
+        <v>42901</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2">
+        <v>8</v>
+      </c>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2">
         <v>7</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3">
-        <v>90.6</v>
-      </c>
-      <c r="F23" s="4">
-        <f t="shared" si="2"/>
-        <v>32.222222222222221</v>
-      </c>
-      <c r="G23" s="3">
-        <v>90</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M23" s="3"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
-        <v>20</v>
-      </c>
-      <c r="B24" s="8">
-        <v>42898</v>
-      </c>
-      <c r="C24" s="5" t="s">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>24</v>
+      </c>
+      <c r="B28" s="7">
+        <v>42902</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>25</v>
+      </c>
+      <c r="B29" s="6">
+        <v>42903</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>26</v>
+      </c>
+      <c r="B30" s="7">
+        <v>42904</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>27</v>
+      </c>
+      <c r="B31" s="6">
+        <v>42905</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5">
-        <v>90.6</v>
-      </c>
-      <c r="F24" s="6">
-        <f t="shared" si="2"/>
-        <v>32.222222222222221</v>
-      </c>
-      <c r="G24" s="5">
-        <v>90</v>
-      </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>28</v>
+      </c>
+      <c r="B32" s="7">
+        <v>42906</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>29</v>
+      </c>
+      <c r="B33" s="6">
+        <v>42907</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>30</v>
+      </c>
+      <c r="B34" s="7">
+        <v>42908</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>31</v>
+      </c>
+      <c r="B35" s="6">
+        <v>42909</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>32</v>
+      </c>
+      <c r="B36" s="7">
+        <v>42910</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>33</v>
+      </c>
+      <c r="B37" s="6">
+        <v>42911</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <v>21</v>
-      </c>
-      <c r="B25" s="7">
-        <v>42899</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3">
-        <v>91.6</v>
-      </c>
-      <c r="F25" s="4">
-        <f t="shared" si="2"/>
-        <v>32.777777777777779</v>
-      </c>
-      <c r="G25" s="3">
-        <v>91</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M25" s="3"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="5">
-        <v>22</v>
-      </c>
-      <c r="B26" s="8">
-        <v>42900</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5">
-        <v>91.6</v>
-      </c>
-      <c r="F26" s="6">
-        <f t="shared" si="2"/>
-        <v>32.777777777777779</v>
-      </c>
-      <c r="G26" s="5">
-        <v>91</v>
-      </c>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B27" s="9"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>-9</v>
-      </c>
-      <c r="B31">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>-2</v>
-      </c>
-      <c r="B32">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>-1</v>
-      </c>
-      <c r="B33">
-        <v>27</v>
-      </c>
-      <c r="C33" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>0</v>
-      </c>
-      <c r="B34">
-        <v>26.999999999999996</v>
-      </c>
-      <c r="C34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <v>27.555555555555554</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>2</v>
-      </c>
-      <c r="B36">
-        <v>27.555555555555554</v>
-      </c>
-      <c r="C36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>3</v>
-      </c>
-      <c r="B37">
-        <v>28.111111111111107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>4</v>
-      </c>
-      <c r="B38">
-        <v>28.111111111111107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>5</v>
-      </c>
-      <c r="B39">
-        <v>28.666666666666668</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>6</v>
-      </c>
-      <c r="B40">
-        <v>28.666666666666668</v>
-      </c>
-      <c r="C40" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>7</v>
-      </c>
-      <c r="B41">
-        <v>29.222222222222221</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>8</v>
-      </c>
-      <c r="B42">
-        <v>29.222222222222221</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>9</v>
-      </c>
-      <c r="B43">
-        <v>29.777777777777779</v>
-      </c>
-      <c r="C43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>10</v>
-      </c>
-      <c r="B44">
-        <v>29.777777777777779</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>11</v>
-      </c>
-      <c r="B45">
-        <v>30.333333333333332</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>12</v>
-      </c>
-      <c r="B46">
-        <v>30.333333333333332</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>13</v>
-      </c>
-      <c r="B47">
-        <v>30.888888888888889</v>
-      </c>
-      <c r="C47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>14</v>
-      </c>
-      <c r="B48">
-        <v>30.888888888888889</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>15</v>
-      </c>
-      <c r="B49">
-        <v>31.444444444444443</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>16</v>
-      </c>
-      <c r="B50">
-        <v>31.444444444444443</v>
-      </c>
-      <c r="C50" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>17</v>
-      </c>
-      <c r="B51">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>18</v>
-      </c>
-      <c r="B52">
-        <v>32</v>
-      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B39" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B13:B27">
-    <cfRule type="timePeriod" dxfId="2" priority="3" timePeriod="today">
-      <formula>FLOOR(B13,1)=TODAY()</formula>
+  <conditionalFormatting sqref="B13:B32 A27:F27 H27">
+    <cfRule type="timePeriod" dxfId="9" priority="10" timePeriod="today">
+      <formula>FLOOR(A13,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F33">
-    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="today">
-      <formula>FLOOR(F33,1)=TODAY()</formula>
+  <conditionalFormatting sqref="A3:M26 J27:M37 A28:M32 I27:M27 G27">
+    <cfRule type="timePeriod" dxfId="8" priority="8" timePeriod="today">
+      <formula>FLOOR(A3,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:M26">
-    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="today">
-      <formula>FLOOR(A3,1)=TODAY()</formula>
+  <conditionalFormatting sqref="B39">
+    <cfRule type="timePeriod" dxfId="7" priority="7" timePeriod="today">
+      <formula>FLOOR(B39,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
+    <cfRule type="timePeriod" dxfId="6" priority="6" timePeriod="today">
+      <formula>FLOOR(B39,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33:B38">
+    <cfRule type="timePeriod" dxfId="5" priority="5" timePeriod="today">
+      <formula>FLOOR(B33,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33:I38">
+    <cfRule type="timePeriod" dxfId="4" priority="4" timePeriod="today">
+      <formula>FLOOR(A33,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J38:M38">
+    <cfRule type="timePeriod" dxfId="3" priority="3" timePeriod="today">
+      <formula>FLOOR(J38,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N37">
+    <cfRule type="timePeriod" dxfId="2" priority="2" timePeriod="today">
+      <formula>FLOOR(N3,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N38">
+    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="today">
+      <formula>FLOOR(N38,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2959,13 +3103,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2992,7 +3136,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3003,7 +3147,7 @@
         <v>26.999999999999996</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3022,7 +3166,7 @@
         <v>27.555555555555554</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -3057,7 +3201,7 @@
         <v>28.666666666666668</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3084,7 +3228,7 @@
         <v>29.777777777777779</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3119,7 +3263,7 @@
         <v>30.888888888888889</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3146,7 +3290,7 @@
         <v>31.444444444444443</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Data through Ipam 9 and T through 19/06/2017.
</commit_message>
<xml_diff>
--- a/ACervStresstestSchedule.xlsx
+++ b/ACervStresstestSchedule.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="94">
   <si>
     <t>Wednesday</t>
   </si>
@@ -284,6 +284,33 @@
   </si>
   <si>
     <t>H 88 Chill 89 @13:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H 88 Chill 89 </t>
+  </si>
+  <si>
+    <t>Y 2 at 90</t>
+  </si>
+  <si>
+    <t>Yes @ 12:30</t>
+  </si>
+  <si>
+    <t>5 microns @ 20:45</t>
+  </si>
+  <si>
+    <t>5 microns @ 16:00</t>
+  </si>
+  <si>
+    <t>5 microns @ 13:00</t>
+  </si>
+  <si>
+    <t>Yes T3</t>
+  </si>
+  <si>
+    <t>Yes Tank 1 moved to Tank 2 from 13:00 to 1630</t>
+  </si>
+  <si>
+    <t>Yes Tank 2 Moved to Tank 1 at 11:40 to 14:20</t>
   </si>
 </sst>
 </file>
@@ -416,7 +443,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -725,11 +772,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-873007120"/>
-        <c:axId val="-873003088"/>
+        <c:axId val="147031472"/>
+        <c:axId val="150022560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-873007120"/>
+        <c:axId val="147031472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,7 +874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-873003088"/>
+        <c:crossAx val="150022560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -835,7 +882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-873003088"/>
+        <c:axId val="150022560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -949,7 +996,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-873007120"/>
+        <c:crossAx val="147031472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1840,10 +1887,10 @@
   <dimension ref="A2:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1856,7 +1903,7 @@
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -2070,9 +2117,8 @@
       <c r="E7" s="2">
         <v>82.6</v>
       </c>
-      <c r="F7" s="3" t="e">
-        <f t="shared" ref="F7:F9" si="1">(G7-32)*5/9</f>
-        <v>#VALUE!</v>
+      <c r="F7" s="3">
+        <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>52</v>
@@ -2106,8 +2152,7 @@
         <v>82.6</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="1"/>
-        <v>27.777777777777779</v>
+        <v>28</v>
       </c>
       <c r="G8" s="4">
         <v>82</v>
@@ -2138,9 +2183,8 @@
       <c r="E9" s="2">
         <v>83.6</v>
       </c>
-      <c r="F9" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="F9" s="3">
+        <v>28.5</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>51</v>
@@ -2174,8 +2218,7 @@
         <v>83.6</v>
       </c>
       <c r="F10" s="5">
-        <f>(G10-32)*5/9</f>
-        <v>28.333333333333332</v>
+        <v>28.5</v>
       </c>
       <c r="G10" s="4">
         <v>83</v>
@@ -2210,9 +2253,8 @@
       <c r="E11" s="2">
         <v>84.6</v>
       </c>
-      <c r="F11" s="3" t="e">
-        <f t="shared" ref="F11:F26" si="2">(G11-32)*5/9</f>
-        <v>#VALUE!</v>
+      <c r="F11" s="3">
+        <v>29</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>49</v>
@@ -2246,8 +2288,7 @@
         <v>84.6</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="2"/>
-        <v>28.888888888888889</v>
+        <v>29</v>
       </c>
       <c r="G12" s="4">
         <v>84</v>
@@ -2282,9 +2323,8 @@
       <c r="E13" s="2">
         <v>85.6</v>
       </c>
-      <c r="F13" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="F13" s="3">
+        <v>29.5</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>50</v>
@@ -2320,8 +2360,7 @@
         <v>85.6</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="2"/>
-        <v>29.444444444444443</v>
+        <v>29.5</v>
       </c>
       <c r="G14" s="4">
         <v>85</v>
@@ -2354,9 +2393,8 @@
       <c r="E15" s="2">
         <v>86.6</v>
       </c>
-      <c r="F15" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="F15" s="3">
+        <v>30</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>44</v>
@@ -2390,7 +2428,6 @@
         <v>86.6</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="G16" s="4">
@@ -2422,9 +2459,8 @@
       <c r="E17" s="2">
         <v>87.6</v>
       </c>
-      <c r="F17" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="F17" s="3">
+        <v>30.5</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>57</v>
@@ -2460,8 +2496,7 @@
         <v>87.6</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="2"/>
-        <v>30</v>
+        <v>30.5</v>
       </c>
       <c r="G18" s="4">
         <v>86</v>
@@ -2494,9 +2529,8 @@
       <c r="E19" s="2">
         <v>88.6</v>
       </c>
-      <c r="F19" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="F19" s="3">
+        <v>31</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>60</v>
@@ -2530,8 +2564,7 @@
         <v>88.6</v>
       </c>
       <c r="F20" s="5">
-        <f t="shared" si="2"/>
-        <v>30.555555555555557</v>
+        <v>31</v>
       </c>
       <c r="G20" s="4">
         <v>87</v>
@@ -2566,9 +2599,8 @@
       <c r="E21" s="2">
         <v>89.6</v>
       </c>
-      <c r="F21" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="F21" s="3">
+        <v>31.5</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>68</v>
@@ -2608,8 +2640,7 @@
         <v>89.6</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="2"/>
-        <v>31.111111111111111</v>
+        <v>31.5</v>
       </c>
       <c r="G22" s="4">
         <v>88</v>
@@ -2642,9 +2673,8 @@
       <c r="E23" s="2">
         <v>90.6</v>
       </c>
-      <c r="F23" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="F23" s="3">
+        <v>32</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>69</v>
@@ -2679,9 +2709,8 @@
       <c r="E24" s="4">
         <v>90.6</v>
       </c>
-      <c r="F24" s="5" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="F24" s="5">
+        <v>32</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>77</v>
@@ -2712,13 +2741,14 @@
       <c r="C25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>32</v>
+      </c>
       <c r="E25" s="2">
         <v>91.6</v>
       </c>
-      <c r="F25" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="F25" s="3">
+        <v>32.5</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>80</v>
@@ -2750,8 +2780,7 @@
         <v>91.6</v>
       </c>
       <c r="F26" s="5">
-        <f t="shared" si="2"/>
-        <v>31.666666666666668</v>
+        <v>32.5</v>
       </c>
       <c r="G26" s="4">
         <v>89</v>
@@ -2782,9 +2811,13 @@
       <c r="C27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>32.5</v>
+      </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3">
+        <v>32.5</v>
+      </c>
       <c r="G27" s="9" t="s">
         <v>84</v>
       </c>
@@ -2796,7 +2829,9 @@
         <v>8</v>
       </c>
       <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
+      <c r="L27" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2">
         <v>7</v>
@@ -2812,17 +2847,31 @@
       <c r="C28" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="4"/>
+      <c r="D28" s="4">
+        <v>32.5</v>
+      </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="F28" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
+      <c r="L28" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+      <c r="N28" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
@@ -2834,17 +2883,27 @@
       <c r="C29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>32.5</v>
+      </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="F29" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="N29" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
@@ -2856,17 +2915,27 @@
       <c r="C30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="4"/>
+      <c r="D30" s="4">
+        <v>32.5</v>
+      </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="F30" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
+      <c r="N30" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
@@ -2878,17 +2947,35 @@
       <c r="C31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>32.5</v>
+      </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="F31" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="J31" s="2">
+        <v>9</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N31" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
@@ -2909,8 +2996,12 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
+      <c r="M32" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N32" s="4">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
@@ -2932,7 +3023,9 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="N33" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
@@ -2954,7 +3047,9 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
+      <c r="N34" s="4">
+        <v>14</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
@@ -2976,7 +3071,9 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+      <c r="N35" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
@@ -3042,49 +3139,64 @@
       <c r="B39" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B13:B32 A27:F27 H27">
-    <cfRule type="timePeriod" dxfId="9" priority="10" timePeriod="today">
+  <conditionalFormatting sqref="B13:B32 A27:C27 H27 E27:F27">
+    <cfRule type="timePeriod" dxfId="11" priority="14" timePeriod="today">
       <formula>FLOOR(A13,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:M26 J27:M37 A28:M32 I27:M27 G27">
-    <cfRule type="timePeriod" dxfId="8" priority="8" timePeriod="today">
+  <conditionalFormatting sqref="A3:M26 J27:M37 I27:M27 G27 A28:M28 A30:M30 A29:E29 A32:M32 A31:E31 G29:M29 G31:M31">
+    <cfRule type="timePeriod" dxfId="10" priority="12" timePeriod="today">
       <formula>FLOOR(A3,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="timePeriod" dxfId="7" priority="7" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="9" priority="11" timePeriod="today">
       <formula>FLOOR(B39,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="timePeriod" dxfId="6" priority="6" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="8" priority="10" timePeriod="today">
       <formula>FLOOR(B39,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:B38">
-    <cfRule type="timePeriod" dxfId="5" priority="5" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="7" priority="9" timePeriod="today">
       <formula>FLOOR(B33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:I38">
-    <cfRule type="timePeriod" dxfId="4" priority="4" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="6" priority="8" timePeriod="today">
       <formula>FLOOR(A33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:M38">
-    <cfRule type="timePeriod" dxfId="3" priority="3" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="5" priority="7" timePeriod="today">
       <formula>FLOOR(J38,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N37">
-    <cfRule type="timePeriod" dxfId="2" priority="2" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="4" priority="6" timePeriod="today">
       <formula>FLOOR(N3,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N38">
-    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="3" priority="5" timePeriod="today">
       <formula>FLOOR(N38,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="timePeriod" dxfId="2" priority="3" timePeriod="today">
+      <formula>FLOOR(D27,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29">
+    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="today">
+      <formula>FLOOR(F29,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F31">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="today">
+      <formula>FLOOR(F31,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Data through 10th Ipam 22/06/2017
</commit_message>
<xml_diff>
--- a/ACervStresstestSchedule.xlsx
+++ b/ACervStresstestSchedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="17900" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="98">
   <si>
     <t>Wednesday</t>
   </si>
@@ -311,6 +311,18 @@
   </si>
   <si>
     <t>Yes Tank 2 Moved to Tank 1 at 11:40 to 14:20</t>
+  </si>
+  <si>
+    <t>T4, 1721, 1738</t>
+  </si>
+  <si>
+    <t>Yes Tank 3 moved to tank 1 and 2 @ 9 to 11:30</t>
+  </si>
+  <si>
+    <t>5 microns @ 15:00</t>
+  </si>
+  <si>
+    <t>T4 all w/o 1725, 1726. T5 1721, 1738 @ 11:30</t>
   </si>
 </sst>
 </file>
@@ -443,7 +455,217 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -772,11 +994,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="147031472"/>
-        <c:axId val="150022560"/>
+        <c:axId val="-2023193216"/>
+        <c:axId val="-2055665856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147031472"/>
+        <c:axId val="-2023193216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +1096,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150022560"/>
+        <c:crossAx val="-2055665856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -882,7 +1104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150022560"/>
+        <c:axId val="-2055665856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,7 +1218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147031472"/>
+        <c:crossAx val="-2023193216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1887,10 +2109,10 @@
   <dimension ref="A2:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomRight" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2987,11 +3209,19 @@
       <c r="C32" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="4"/>
+      <c r="D32" s="4">
+        <v>32.5</v>
+      </c>
       <c r="E32" s="4"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="F32" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -3013,16 +3243,32 @@
       <c r="C33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2">
+        <v>32.5</v>
+      </c>
       <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+      <c r="F33" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J33" s="2">
+        <v>10</v>
+      </c>
       <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
+      <c r="L33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="N33" s="2">
         <v>13</v>
       </c>
@@ -3037,14 +3283,26 @@
       <c r="C34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="4"/>
+      <c r="D34" s="4">
+        <v>32.5</v>
+      </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="F34" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="K34" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4">
@@ -3061,13 +3319,23 @@
       <c r="C35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2">
+        <v>32.5</v>
+      </c>
       <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="F35" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+      <c r="J35" s="2">
+        <v>11</v>
+      </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
@@ -3085,17 +3353,27 @@
       <c r="C36" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="4"/>
+      <c r="D36" s="4">
+        <v>32.5</v>
+      </c>
       <c r="E36" s="4"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+      <c r="F36" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
+      <c r="N36" s="4">
+        <v>16</v>
+      </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
@@ -3109,15 +3387,23 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
+      <c r="F37" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+      <c r="N37" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
@@ -3133,70 +3419,132 @@
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
+      <c r="N38" s="4">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B39" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B13:B32 A27:C27 H27 E27:F27">
-    <cfRule type="timePeriod" dxfId="11" priority="14" timePeriod="today">
+  <conditionalFormatting sqref="B13:B32 A27:C27 H27 E27:F27 J33:K33 M33">
+    <cfRule type="timePeriod" dxfId="32" priority="26" timePeriod="today">
       <formula>FLOOR(A13,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:M26 J27:M37 I27:M27 G27 A28:M28 A30:M30 A29:E29 A32:M32 A31:E31 G29:M29 G31:M31">
-    <cfRule type="timePeriod" dxfId="10" priority="12" timePeriod="today">
+  <conditionalFormatting sqref="A3:M26 J27:M32 I27:M27 G27 A28:M28 A30:M30 A29:E29 A31:E31 G29:M29 G31:M31 A32:G32 I32:M32 J34:M37">
+    <cfRule type="timePeriod" dxfId="31" priority="24" timePeriod="today">
       <formula>FLOOR(A3,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="timePeriod" dxfId="9" priority="11" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="30" priority="23" timePeriod="today">
       <formula>FLOOR(B39,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="timePeriod" dxfId="8" priority="10" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="29" priority="22" timePeriod="today">
       <formula>FLOOR(B39,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:B38">
-    <cfRule type="timePeriod" dxfId="7" priority="9" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="28" priority="21" timePeriod="today">
       <formula>FLOOR(B33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33:I38">
-    <cfRule type="timePeriod" dxfId="6" priority="8" timePeriod="today">
+  <conditionalFormatting sqref="A34:E34 A33:F33 A38:I38 A35:C36 E35:E36 A37:E37 I33:I37">
+    <cfRule type="timePeriod" dxfId="27" priority="20" timePeriod="today">
       <formula>FLOOR(A33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:M38">
-    <cfRule type="timePeriod" dxfId="5" priority="7" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="26" priority="19" timePeriod="today">
       <formula>FLOOR(J38,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N37">
-    <cfRule type="timePeriod" dxfId="4" priority="6" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="25" priority="18" timePeriod="today">
       <formula>FLOOR(N3,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N38">
-    <cfRule type="timePeriod" dxfId="3" priority="5" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="24" priority="17" timePeriod="today">
       <formula>FLOOR(N38,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="timePeriod" dxfId="2" priority="3" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="23" priority="15" timePeriod="today">
       <formula>FLOOR(D27,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="22" priority="14" timePeriod="today">
       <formula>FLOOR(F29,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="21" priority="13" timePeriod="today">
       <formula>FLOOR(F31,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33">
+    <cfRule type="timePeriod" dxfId="20" priority="12" timePeriod="today">
+      <formula>FLOOR(G33,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32:H33">
+    <cfRule type="timePeriod" dxfId="19" priority="11" timePeriod="today">
+      <formula>FLOOR(H32,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L33">
+    <cfRule type="timePeriod" dxfId="18" priority="10" timePeriod="today">
+      <formula>FLOOR(L33,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:D36">
+    <cfRule type="timePeriod" dxfId="17" priority="9" timePeriod="today">
+      <formula>FLOOR(D35,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F34:G34">
+    <cfRule type="timePeriod" dxfId="15" priority="8" timePeriod="today">
+      <formula>FLOOR(F34,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35">
+    <cfRule type="timePeriod" dxfId="13" priority="7" timePeriod="today">
+      <formula>FLOOR(F35,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="timePeriod" dxfId="11" priority="6" timePeriod="today">
+      <formula>FLOOR(G35,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:H35">
+    <cfRule type="timePeriod" dxfId="9" priority="5" timePeriod="today">
+      <formula>FLOOR(H34,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36:G36">
+    <cfRule type="timePeriod" dxfId="7" priority="4" timePeriod="today">
+      <formula>FLOOR(F36,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F37">
+    <cfRule type="timePeriod" dxfId="5" priority="3" timePeriod="today">
+      <formula>FLOOR(F37,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G37">
+    <cfRule type="timePeriod" dxfId="3" priority="2" timePeriod="today">
+      <formula>FLOOR(G37,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36:H37">
+    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="today">
+      <formula>FLOOR(H36,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Data through 26/06/2017.  The 12th Ipam
</commit_message>
<xml_diff>
--- a/ACervStresstestSchedule.xlsx
+++ b/ACervStresstestSchedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17900" tabRatio="500"/>
+    <workbookView xWindow="4720" yWindow="0" windowWidth="24080" windowHeight="17900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="104">
   <si>
     <t>Wednesday</t>
   </si>
@@ -323,6 +323,24 @@
   </si>
   <si>
     <t>T4 all w/o 1725, 1726. T5 1721, 1738 @ 11:30</t>
+  </si>
+  <si>
+    <t>H 88 Chill 89</t>
+  </si>
+  <si>
+    <t>5 microns @ 9:30</t>
+  </si>
+  <si>
+    <t>5 microns @ 14:30</t>
+  </si>
+  <si>
+    <t>5 microns @ 14:00</t>
+  </si>
+  <si>
+    <t>T6 @ 15:00</t>
+  </si>
+  <si>
+    <t>T6/T7 1721, 1732, 1734, 1738</t>
   </si>
 </sst>
 </file>
@@ -352,7 +370,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,12 +392,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -445,9 +457,6 @@
     <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,137 +464,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -905,6 +784,39 @@
                 <c:pt idx="6">
                   <c:v>Sunday</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Friday</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Saturday</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Sunday</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Thursday</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -950,6 +862,39 @@
                 <c:pt idx="6">
                   <c:v>33.0</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -979,6 +924,39 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>42911.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42912.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42913.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42914.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42915.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42916.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42917.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42918.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42919.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42920.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42921.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42922.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -994,11 +972,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2023193216"/>
-        <c:axId val="-2055665856"/>
+        <c:axId val="-469243648"/>
+        <c:axId val="-469239616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2023193216"/>
+        <c:axId val="-469243648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1096,7 +1074,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055665856"/>
+        <c:crossAx val="-469239616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1104,7 +1082,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2055665856"/>
+        <c:axId val="-469239616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1218,7 +1196,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2023193216"/>
+        <c:crossAx val="-469243648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2106,13 +2084,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N39"/>
+  <dimension ref="A2:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="I9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K35" sqref="K35"/>
+      <selection pane="bottomRight" activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3040,7 +3018,7 @@
       <c r="F27" s="3">
         <v>32.5</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="8" t="s">
         <v>84</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -3112,7 +3090,7 @@
       <c r="F29" s="3">
         <v>32.5</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="8" t="s">
         <v>85</v>
       </c>
       <c r="H29" s="2" t="s">
@@ -3176,7 +3154,7 @@
       <c r="F31" s="3">
         <v>32.5</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="8" t="s">
         <v>85</v>
       </c>
       <c r="H31" s="2" t="s">
@@ -3250,7 +3228,7 @@
       <c r="F33" s="3">
         <v>32.5</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="8" t="s">
         <v>85</v>
       </c>
       <c r="H33" s="2" t="s">
@@ -3326,7 +3304,7 @@
       <c r="F35" s="3">
         <v>32.5</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G35" s="8" t="s">
         <v>85</v>
       </c>
       <c r="H35" s="2" t="s">
@@ -3337,7 +3315,9 @@
         <v>11</v>
       </c>
       <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
+      <c r="L35" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2">
         <v>15</v>
@@ -3366,10 +3346,14 @@
       <c r="H36" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
+      <c r="L36" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4">
         <v>16</v>
@@ -3385,18 +3369,22 @@
       <c r="C37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="2"/>
+      <c r="D37" s="2">
+        <v>32.5</v>
+      </c>
       <c r="E37" s="2"/>
       <c r="F37" s="3">
         <v>32.5</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="8" t="s">
         <v>85</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I37" s="2"/>
+      <c r="I37" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -3406,144 +3394,459 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
+      <c r="A38" s="4">
+        <v>34</v>
+      </c>
+      <c r="B38" s="7">
+        <v>42912</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="4">
+        <v>32.5</v>
+      </c>
       <c r="E38" s="4"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
+      <c r="F38" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
+      <c r="J38" s="4">
+        <v>12</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="M38" s="4"/>
       <c r="N38" s="4">
         <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B39" s="8"/>
+      <c r="A39" s="2">
+        <v>35</v>
+      </c>
+      <c r="B39" s="6">
+        <v>42913</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>36</v>
+      </c>
+      <c r="B40" s="7">
+        <v>42914</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>37</v>
+      </c>
+      <c r="B41" s="7">
+        <v>42915</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>38</v>
+      </c>
+      <c r="B42" s="6">
+        <v>42916</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>39</v>
+      </c>
+      <c r="B43" s="7">
+        <v>42917</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>40</v>
+      </c>
+      <c r="B44" s="6">
+        <v>42918</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
+        <v>41</v>
+      </c>
+      <c r="B45" s="7">
+        <v>42919</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>42</v>
+      </c>
+      <c r="B46" s="6">
+        <v>42920</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>43</v>
+      </c>
+      <c r="B47" s="7">
+        <v>42921</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>44</v>
+      </c>
+      <c r="B48" s="6">
+        <v>42922</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B13:B32 A27:C27 H27 E27:F27 J33:K33 M33">
-    <cfRule type="timePeriod" dxfId="32" priority="26" timePeriod="today">
+  <conditionalFormatting sqref="B13:B32 A27:C27 H27 E27:F27 J33:K33 M33 B38 J39:K39 M39 B41 J42:K42 M42 B47 J48:K48 M48">
+    <cfRule type="timePeriod" dxfId="19" priority="26" timePeriod="today">
       <formula>FLOOR(A13,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:M26 J27:M32 I27:M27 G27 A28:M28 A30:M30 A29:E29 A31:E31 G29:M29 G31:M31 A32:G32 I32:M32 J34:M37">
-    <cfRule type="timePeriod" dxfId="31" priority="24" timePeriod="today">
+  <conditionalFormatting sqref="A3:M26 J27:M32 I27:M27 G27 A28:M28 A30:M30 A29:E29 A31:E31 G29:M29 G31:M31 A32:G32 I32:M32 J34:M37 A38:G38 I38:M38 J40:M40 A41:G41 I41:M41 J43:M46 A47:G47 I47:M47">
+    <cfRule type="timePeriod" dxfId="18" priority="24" timePeriod="today">
       <formula>FLOOR(A3,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="timePeriod" dxfId="30" priority="23" timePeriod="today">
-      <formula>FLOOR(B39,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="timePeriod" dxfId="29" priority="22" timePeriod="today">
-      <formula>FLOOR(B39,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:B38">
-    <cfRule type="timePeriod" dxfId="28" priority="21" timePeriod="today">
+  <conditionalFormatting sqref="B33:B37 B39:B40 B42:B46 B48">
+    <cfRule type="timePeriod" dxfId="17" priority="21" timePeriod="today">
       <formula>FLOOR(B33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A34:E34 A33:F33 A38:I38 A35:C36 E35:E36 A37:E37 I33:I37">
-    <cfRule type="timePeriod" dxfId="27" priority="20" timePeriod="today">
+  <conditionalFormatting sqref="A34:E34 A33:F33 A35:C36 E35:E36 A37:E37 I33:I37 A40:E40 A39:F39 I39:I40 A43:E43 A42:F42 A44:C45 E44:E45 A46:E46 I42:I46 A48:F48 I48">
+    <cfRule type="timePeriod" dxfId="16" priority="20" timePeriod="today">
       <formula>FLOOR(A33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J38:M38">
-    <cfRule type="timePeriod" dxfId="26" priority="19" timePeriod="today">
-      <formula>FLOOR(J38,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N37">
-    <cfRule type="timePeriod" dxfId="25" priority="18" timePeriod="today">
+  <conditionalFormatting sqref="N3:N48">
+    <cfRule type="timePeriod" dxfId="15" priority="18" timePeriod="today">
       <formula>FLOOR(N3,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N38">
-    <cfRule type="timePeriod" dxfId="24" priority="17" timePeriod="today">
-      <formula>FLOOR(N38,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="timePeriod" dxfId="23" priority="15" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="14" priority="15" timePeriod="today">
       <formula>FLOOR(D27,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="timePeriod" dxfId="22" priority="14" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="13" priority="14" timePeriod="today">
       <formula>FLOOR(F29,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="timePeriod" dxfId="21" priority="13" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="12" priority="13" timePeriod="today">
       <formula>FLOOR(F31,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
-    <cfRule type="timePeriod" dxfId="20" priority="12" timePeriod="today">
+  <conditionalFormatting sqref="G33 G39 G42 G48">
+    <cfRule type="timePeriod" dxfId="11" priority="12" timePeriod="today">
       <formula>FLOOR(G33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32:H33">
-    <cfRule type="timePeriod" dxfId="19" priority="11" timePeriod="today">
+  <conditionalFormatting sqref="H32:H33 H38:H39 H41:H42 H47:H48">
+    <cfRule type="timePeriod" dxfId="10" priority="11" timePeriod="today">
       <formula>FLOOR(H32,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L33">
-    <cfRule type="timePeriod" dxfId="18" priority="10" timePeriod="today">
+  <conditionalFormatting sqref="L33 L39 L42 L48">
+    <cfRule type="timePeriod" dxfId="9" priority="10" timePeriod="today">
       <formula>FLOOR(L33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D36">
-    <cfRule type="timePeriod" dxfId="17" priority="9" timePeriod="today">
+  <conditionalFormatting sqref="D35:D36 D44:D45">
+    <cfRule type="timePeriod" dxfId="8" priority="9" timePeriod="today">
       <formula>FLOOR(D35,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34:G34">
-    <cfRule type="timePeriod" dxfId="15" priority="8" timePeriod="today">
+  <conditionalFormatting sqref="F34:G34 F40:G40 F43:G43">
+    <cfRule type="timePeriod" dxfId="7" priority="8" timePeriod="today">
       <formula>FLOOR(F34,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
-    <cfRule type="timePeriod" dxfId="13" priority="7" timePeriod="today">
+  <conditionalFormatting sqref="F35 F44">
+    <cfRule type="timePeriod" dxfId="6" priority="7" timePeriod="today">
       <formula>FLOOR(F35,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="timePeriod" dxfId="11" priority="6" timePeriod="today">
+  <conditionalFormatting sqref="G35 G44">
+    <cfRule type="timePeriod" dxfId="5" priority="6" timePeriod="today">
       <formula>FLOOR(G35,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34:H35">
-    <cfRule type="timePeriod" dxfId="9" priority="5" timePeriod="today">
+  <conditionalFormatting sqref="H34:H35 H40 H43:H44">
+    <cfRule type="timePeriod" dxfId="4" priority="5" timePeriod="today">
       <formula>FLOOR(H34,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F36:G36">
-    <cfRule type="timePeriod" dxfId="7" priority="4" timePeriod="today">
+  <conditionalFormatting sqref="F36:G36 F45:G45">
+    <cfRule type="timePeriod" dxfId="3" priority="4" timePeriod="today">
       <formula>FLOOR(F36,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F37">
-    <cfRule type="timePeriod" dxfId="5" priority="3" timePeriod="today">
+  <conditionalFormatting sqref="F37 F46">
+    <cfRule type="timePeriod" dxfId="2" priority="3" timePeriod="today">
       <formula>FLOOR(F37,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
-    <cfRule type="timePeriod" dxfId="3" priority="2" timePeriod="today">
+  <conditionalFormatting sqref="G37 G46">
+    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="today">
       <formula>FLOOR(G37,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36:H37">
-    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="today">
+  <conditionalFormatting sqref="H36:H37 H45:H46">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="today">
       <formula>FLOOR(H36,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
R Data and scripts
</commit_message>
<xml_diff>
--- a/ACervStresstestSchedule.xlsx
+++ b/ACervStresstestSchedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8440" yWindow="0" windowWidth="20360" windowHeight="17900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Stress" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="144">
   <si>
     <t>Wednesday</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Change Filter</t>
   </si>
   <si>
-    <t>0 Actual Day 12</t>
-  </si>
-  <si>
     <t>Initial</t>
   </si>
   <si>
@@ -420,7 +417,49 @@
     <t>5 micons @ 16:30</t>
   </si>
   <si>
-    <t>Added HOBO T probe at 15:10, Pumps still on all the time</t>
+    <t>Added HOBO T2 probe at 15:10, Pumps still on all the time</t>
+  </si>
+  <si>
+    <t>1st Recovery</t>
+  </si>
+  <si>
+    <t>Yes @ 13:20</t>
+  </si>
+  <si>
+    <t>5 micron @ 14:00</t>
+  </si>
+  <si>
+    <t>Relabel</t>
+  </si>
+  <si>
+    <t>Polyps P0 @10:30</t>
+  </si>
+  <si>
+    <t>Yes @ 14:20</t>
+  </si>
+  <si>
+    <t>T5 @ 15:00</t>
+  </si>
+  <si>
+    <t>5 Micron @ 9:15</t>
+  </si>
+  <si>
+    <t>Yes @ 18:00</t>
+  </si>
+  <si>
+    <t>Added HOBO T1, T3, probe at 15:30, Pumps still on all the time. All HOBO online by 16:15 logging every 15 minutes. Have approxmiately 36 days of data</t>
+  </si>
+  <si>
+    <t>2nd Recovery (16)</t>
+  </si>
+  <si>
+    <t>Polyps P1 @12 and 4 Mcavs</t>
+  </si>
+  <si>
+    <t>5 Micron @ 13:15</t>
+  </si>
+  <si>
+    <t>1 Actual Day 12</t>
   </si>
 </sst>
 </file>
@@ -590,7 +629,297 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="99">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1566,11 +1895,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="G19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="H20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I54" sqref="I54"/>
+      <selection pane="bottomRight" activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1601,19 +1930,19 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>12</v>
@@ -1628,10 +1957,10 @@
         <v>15</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1658,22 +1987,22 @@
         <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>143</v>
       </c>
       <c r="B4" s="7">
         <v>42878</v>
@@ -1689,19 +2018,19 @@
         <v>80.599999999999994</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" ref="F4:F6" si="0">(E4-32)*5/9</f>
+        <f>(E4-32)*5/9</f>
         <v>26.999999999999996</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -1709,7 +2038,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="6">
         <v>42879</v>
@@ -1718,35 +2047,35 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2">
         <v>81.599999999999994</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="0"/>
+        <f>(E5-32)*5/9</f>
         <v>27.555555555555554</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="7">
         <v>42880</v>
@@ -1755,27 +2084,27 @@
         <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="4">
         <v>81.599999999999994</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" si="0"/>
+        <f>(E6-32)*5/9</f>
         <v>27.555555555555554</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4">
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -1783,7 +2112,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="6">
         <v>42881</v>
@@ -1792,7 +2121,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2">
         <v>82.6</v>
@@ -1801,23 +2130,23 @@
         <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7">
         <v>42882</v>
@@ -1826,7 +2155,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="4">
         <v>82.6</v>
@@ -1838,7 +2167,7 @@
         <v>82</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1849,7 +2178,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="6">
         <v>42883</v>
@@ -1858,7 +2187,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2">
         <v>83.6</v>
@@ -1867,23 +2196,23 @@
         <v>28.5</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" s="7">
         <v>42884</v>
@@ -1892,7 +2221,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="4">
         <v>83.6</v>
@@ -1904,14 +2233,14 @@
         <v>83</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4">
         <v>3</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -1919,7 +2248,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="6">
         <v>42885</v>
@@ -1937,23 +2266,23 @@
         <v>29</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="7">
         <v>42886</v>
@@ -1962,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4">
         <v>84.6</v>
@@ -1974,22 +2303,22 @@
         <v>84</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="6">
         <v>42887</v>
@@ -1997,8 +2326,8 @@
       <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>49</v>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E13" s="2">
         <v>85.6</v>
@@ -2007,10 +2336,10 @@
         <v>29.5</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2">
@@ -2018,14 +2347,14 @@
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" s="7">
         <v>42888</v>
@@ -2034,7 +2363,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" s="4">
         <v>85.6</v>
@@ -2046,10 +2375,10 @@
         <v>85</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2059,7 +2388,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="6">
         <v>42889</v>
@@ -2068,7 +2397,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2">
         <v>86.6</v>
@@ -2077,23 +2406,23 @@
         <v>30</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="7">
         <v>42890</v>
@@ -2102,7 +2431,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="4">
         <v>86.6</v>
@@ -2114,7 +2443,7 @@
         <v>86</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -2125,7 +2454,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="6">
         <v>42891</v>
@@ -2134,7 +2463,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2">
         <v>87.6</v>
@@ -2143,10 +2472,10 @@
         <v>30.5</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2">
@@ -2154,14 +2483,14 @@
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="7">
         <v>42892</v>
@@ -2170,7 +2499,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="4">
         <v>87.6</v>
@@ -2182,12 +2511,12 @@
         <v>86</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -2195,7 +2524,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="6">
         <v>42893</v>
@@ -2204,7 +2533,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="2">
         <v>88.6</v>
@@ -2213,23 +2542,23 @@
         <v>31</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" s="7">
         <v>42894</v>
@@ -2238,7 +2567,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="4">
         <v>88.6</v>
@@ -2250,7 +2579,7 @@
         <v>87</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4">
@@ -2258,14 +2587,14 @@
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" s="6">
         <v>42895</v>
@@ -2274,7 +2603,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="2">
         <v>89.6</v>
@@ -2283,20 +2612,20 @@
         <v>31.5</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2">
@@ -2305,7 +2634,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="7">
         <v>42896</v>
@@ -2314,7 +2643,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="4">
         <v>89.6</v>
@@ -2326,7 +2655,7 @@
         <v>88</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -2339,7 +2668,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" s="6">
         <v>42897</v>
@@ -2348,7 +2677,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="2">
         <v>90.6</v>
@@ -2357,16 +2686,16 @@
         <v>32</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2">
@@ -2375,7 +2704,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B24" s="7">
         <v>42898</v>
@@ -2393,10 +2722,10 @@
         <v>32</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4">
@@ -2404,7 +2733,7 @@
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4">
@@ -2413,7 +2742,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" s="6">
         <v>42899</v>
@@ -2431,7 +2760,7 @@
         <v>32.5</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -2445,7 +2774,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B26" s="7">
         <v>42900</v>
@@ -2454,7 +2783,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E26" s="4">
         <v>91.6</v>
@@ -2466,15 +2795,15 @@
         <v>89</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4">
@@ -2483,7 +2812,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B27" s="6">
         <v>42901</v>
@@ -2499,10 +2828,10 @@
         <v>32.5</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2">
@@ -2510,7 +2839,7 @@
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2">
@@ -2519,7 +2848,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B28" s="7">
         <v>42902</v>
@@ -2535,18 +2864,18 @@
         <v>32.5</v>
       </c>
       <c r="G28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H28" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="I28" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4">
@@ -2555,7 +2884,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B29" s="6">
         <v>42903</v>
@@ -2571,10 +2900,10 @@
         <v>32.5</v>
       </c>
       <c r="G29" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -2587,7 +2916,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30" s="7">
         <v>42904</v>
@@ -2603,10 +2932,10 @@
         <v>32.5</v>
       </c>
       <c r="G30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -2619,7 +2948,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B31" s="6">
         <v>42905</v>
@@ -2635,23 +2964,23 @@
         <v>32.5</v>
       </c>
       <c r="G31" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2">
         <v>9</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N31" s="2">
         <v>11</v>
@@ -2659,7 +2988,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B32" s="7">
         <v>42906</v>
@@ -2675,17 +3004,19 @@
         <v>32.5</v>
       </c>
       <c r="G32" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H32" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N32" s="4">
         <v>12</v>
@@ -2693,7 +3024,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B33" s="6">
         <v>42907</v>
@@ -2709,23 +3040,21 @@
         <v>32.5</v>
       </c>
       <c r="G33" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>88</v>
-      </c>
+      <c r="I33" s="2"/>
       <c r="J33" s="2">
         <v>10</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N33" s="2">
         <v>13</v>
@@ -2733,7 +3062,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B34" s="7">
         <v>42908</v>
@@ -2749,17 +3078,17 @@
         <v>32.5</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H34" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="I34" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -2769,7 +3098,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B35" s="6">
         <v>42909</v>
@@ -2785,10 +3114,10 @@
         <v>32.5</v>
       </c>
       <c r="G35" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2">
@@ -2796,7 +3125,7 @@
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2">
@@ -2805,7 +3134,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B36" s="7">
         <v>42910</v>
@@ -2821,18 +3150,18 @@
         <v>32.5</v>
       </c>
       <c r="G36" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H36" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="I36" s="4" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4">
@@ -2841,7 +3170,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B37" s="6">
         <v>42911</v>
@@ -2857,13 +3186,13 @@
         <v>32.5</v>
       </c>
       <c r="G37" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="I37" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -2875,7 +3204,7 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B38" s="7">
         <v>42912</v>
@@ -2891,20 +3220,20 @@
         <v>32.5</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4">
         <v>12</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="4">
@@ -2913,7 +3242,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B39" s="6">
         <v>42913</v>
@@ -2929,13 +3258,13 @@
         <v>32.5</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -2946,8 +3275,8 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
-        <v>36</v>
+      <c r="A40" s="2">
+        <v>37</v>
       </c>
       <c r="B40" s="7">
         <v>42914</v>
@@ -2963,10 +3292,10 @@
         <v>32.5</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4">
@@ -2981,7 +3310,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B41" s="7">
         <v>42915</v>
@@ -2997,20 +3326,20 @@
         <v>32.5</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M41" s="4"/>
       <c r="N41" s="4">
@@ -3019,7 +3348,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B42" s="6">
         <v>42916</v>
@@ -3035,10 +3364,10 @@
         <v>32.5</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2">
@@ -3046,19 +3375,19 @@
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2">
         <v>22</v>
       </c>
       <c r="O42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B43" s="7">
         <v>42917</v>
@@ -3074,30 +3403,30 @@
         <v>32.5</v>
       </c>
       <c r="G43" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H43" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="I43" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M43" s="4"/>
       <c r="N43" s="4">
         <v>23</v>
       </c>
       <c r="O43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B44" s="6">
         <v>42918</v>
@@ -3113,10 +3442,10 @@
         <v>26.5</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -3127,7 +3456,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B45" s="7">
         <v>42919</v>
@@ -3143,23 +3472,23 @@
         <v>26.5</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -3179,108 +3508,108 @@
   <mergeCells count="1">
     <mergeCell ref="A46:N46"/>
   </mergeCells>
-  <conditionalFormatting sqref="B13:B32 A27:C27 H27 E27:F27 J33:K33 M33 B38 J39:K39 M39 B41 J42:K42 M42">
-    <cfRule type="timePeriod" dxfId="69" priority="27" timePeriod="today">
-      <formula>FLOOR(A13,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:M26 J27:M32 I27:M27 G27 A28:M28 A30:M30 A29:E29 A31:E31 G29:M29 G31:M31 A32:G32 I32:M32 J34:M37 A38:G38 I38:M38 J40:M40 A41:G41 I41:M41 J43:M45">
-    <cfRule type="timePeriod" dxfId="68" priority="25" timePeriod="today">
+  <conditionalFormatting sqref="B13:B32 B27:C27 H27 E27:F27 J33:K33 M33 B38 J39:K39 M39 B41 J42:K42 M42">
+    <cfRule type="timePeriod" dxfId="98" priority="27" timePeriod="today">
+      <formula>FLOOR(B13,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:M8 J27:M32 I27:M27 G27 B28:M28 B30:M30 B29:E29 B31:E31 G29:M29 G31:M31 B32:G32 I32:M32 J34:M37 B38:G38 I38:M38 J40:M40 B41:G41 I41:M41 J43:M45 A9:A45 B9:M26">
+    <cfRule type="timePeriod" dxfId="97" priority="25" timePeriod="today">
       <formula>FLOOR(A3,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:B37 B39:B40 B42:B45">
-    <cfRule type="timePeriod" dxfId="67" priority="22" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="96" priority="22" timePeriod="today">
       <formula>FLOOR(B33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A34:E34 A33:F33 A35:C36 E35:E36 A37:E37 I33:I37 A40:E40 A39:F39 I39:I40 A43:E43 A42:F42 A44:C45 E44:E45 A46 I42:I45">
-    <cfRule type="timePeriod" dxfId="66" priority="21" timePeriod="today">
+  <conditionalFormatting sqref="B34:E34 B33:F33 B35:C36 E35:E36 B37:E37 I33:I37 B40:E40 B39:F39 I39:I40 B43:E43 B42:F42 B44:C45 E44:E45 A46 I42:I45">
+    <cfRule type="timePeriod" dxfId="95" priority="21" timePeriod="today">
       <formula>FLOOR(A33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N45">
-    <cfRule type="timePeriod" dxfId="65" priority="19" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="94" priority="19" timePeriod="today">
       <formula>FLOOR(N3,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="timePeriod" dxfId="64" priority="16" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="93" priority="16" timePeriod="today">
       <formula>FLOOR(D27,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="timePeriod" dxfId="63" priority="15" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="92" priority="15" timePeriod="today">
       <formula>FLOOR(F29,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="timePeriod" dxfId="62" priority="14" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="91" priority="14" timePeriod="today">
       <formula>FLOOR(F31,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33 G39 G42">
-    <cfRule type="timePeriod" dxfId="61" priority="13" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="90" priority="13" timePeriod="today">
       <formula>FLOOR(G33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H33 H38:H39 H41:H42">
-    <cfRule type="timePeriod" dxfId="60" priority="12" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="89" priority="12" timePeriod="today">
       <formula>FLOOR(H32,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33 L39 L42">
-    <cfRule type="timePeriod" dxfId="59" priority="11" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="88" priority="11" timePeriod="today">
       <formula>FLOOR(L33,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D36 D44:D45">
-    <cfRule type="timePeriod" dxfId="58" priority="10" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="87" priority="10" timePeriod="today">
       <formula>FLOOR(D35,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:G34 F40:G40 F43:G43">
-    <cfRule type="timePeriod" dxfId="57" priority="9" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="86" priority="9" timePeriod="today">
       <formula>FLOOR(F34,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="timePeriod" dxfId="56" priority="8" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="85" priority="8" timePeriod="today">
       <formula>FLOOR(F35,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35 G44">
-    <cfRule type="timePeriod" dxfId="55" priority="7" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="84" priority="7" timePeriod="today">
       <formula>FLOOR(G35,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34:H35 H40 H43:H44">
-    <cfRule type="timePeriod" dxfId="54" priority="6" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="83" priority="6" timePeriod="today">
       <formula>FLOOR(H34,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36:G36 G45">
-    <cfRule type="timePeriod" dxfId="53" priority="5" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="82" priority="5" timePeriod="today">
       <formula>FLOOR(F36,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37">
-    <cfRule type="timePeriod" dxfId="52" priority="4" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="81" priority="4" timePeriod="today">
       <formula>FLOOR(F37,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="timePeriod" dxfId="51" priority="3" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="80" priority="3" timePeriod="today">
       <formula>FLOOR(G37,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:H37 H45">
-    <cfRule type="timePeriod" dxfId="50" priority="2" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="79" priority="2" timePeriod="today">
       <formula>FLOOR(H36,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:F45">
-    <cfRule type="timePeriod" dxfId="49" priority="1" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="78" priority="1" timePeriod="today">
       <formula>FLOOR(F44,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3292,8 +3621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3313,16 +3642,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>12</v>
@@ -3337,13 +3666,13 @@
         <v>15</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -3368,7 +3697,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N2" s="2"/>
     </row>
@@ -3463,7 +3792,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -3516,7 +3845,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N8" s="2"/>
     </row>
@@ -3563,22 +3892,22 @@
         <v>27</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N10" s="2">
         <v>2</v>
@@ -3601,10 +3930,10 @@
         <v>27</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -3633,20 +3962,20 @@
         <v>27</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -3671,17 +4000,17 @@
         <v>27</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4">
@@ -3705,21 +4034,21 @@
         <v>27</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2">
@@ -3743,10 +4072,10 @@
         <v>27</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -3775,10 +4104,10 @@
         <v>27</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3807,24 +4136,24 @@
         <v>27</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L17" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M17" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="N17" s="4">
         <v>9</v>
@@ -3847,10 +4176,10 @@
         <v>27</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -3879,26 +4208,26 @@
         <v>27</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4">
         <v>11</v>
       </c>
       <c r="O19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -3914,11 +4243,19 @@
       <c r="D20" s="2">
         <v>27</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="2"/>
+      <c r="E20" s="3">
+        <v>27</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -3926,6 +4263,9 @@
       <c r="N20" s="2">
         <v>12</v>
       </c>
+      <c r="O20" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
@@ -3940,15 +4280,31 @@
       <c r="D21" s="4">
         <v>27</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="E21" s="5">
+        <v>27</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
+      <c r="J21" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="N21" s="4">
         <v>13</v>
       </c>
@@ -3966,9 +4322,15 @@
       <c r="D22" s="2">
         <v>27</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="2"/>
+      <c r="E22" s="3">
+        <v>27</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -3992,9 +4354,15 @@
       <c r="D23" s="4">
         <v>27</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="E23" s="5">
+        <v>27</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -4007,121 +4375,241 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="B24" s="6">
+        <v>42933</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="2">
+        <v>27</v>
+      </c>
+      <c r="E24" s="3">
+        <v>27</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
+      <c r="N24" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="B25" s="7">
+        <v>42934</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="4">
+        <v>27</v>
+      </c>
+      <c r="E25" s="5">
+        <v>27</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="J25" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
+      <c r="N25" s="4">
+        <v>17</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="2"/>
+      <c r="B26" s="6">
+        <v>42935</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>27</v>
+      </c>
+      <c r="E26" s="3">
+        <v>27</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
+      <c r="K26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="N26" s="2">
+        <v>18</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="B27" s="7">
+        <v>42936</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4">
+        <v>27</v>
+      </c>
+      <c r="E27" s="5">
+        <v>27</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="I27" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
+      <c r="N27" s="4">
+        <v>19</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="B28" s="6">
+        <v>42937</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2">
+        <v>27</v>
+      </c>
+      <c r="E28" s="3">
+        <v>27</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
+      <c r="K28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="N28" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="B29" s="7">
+        <v>42938</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="4">
+        <v>27</v>
+      </c>
+      <c r="E29" s="5">
+        <v>27</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+      <c r="N29" s="4">
+        <v>21</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="2"/>
+      <c r="B30" s="6">
+        <v>42939</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="2">
+        <v>27</v>
+      </c>
+      <c r="E30" s="3">
+        <v>27</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="N30" s="2">
+        <v>22</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="7">
+        <v>42940</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="4">
+        <v>27</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -4131,13 +4619,21 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
+      <c r="N31" s="4">
+        <v>23</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3"/>
+      <c r="B32" s="6">
+        <v>42941</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="2">
+        <v>27</v>
+      </c>
       <c r="E32" s="3"/>
       <c r="F32" s="8"/>
       <c r="G32" s="2"/>
@@ -4151,9 +4647,15 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
+      <c r="B33" s="7">
+        <v>42942</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <v>27</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -4167,9 +4669,15 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3"/>
+      <c r="B34" s="6">
+        <v>42943</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>27</v>
+      </c>
       <c r="E34" s="3"/>
       <c r="F34" s="8"/>
       <c r="G34" s="2"/>
@@ -4183,9 +4691,15 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
+      <c r="B35" s="7">
+        <v>42944</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="4">
+        <v>27</v>
+      </c>
       <c r="E35" s="5"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -4199,9 +4713,15 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
+      <c r="B36" s="6">
+        <v>42945</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2">
+        <v>27</v>
+      </c>
       <c r="E36" s="3"/>
       <c r="F36" s="8"/>
       <c r="G36" s="2"/>
@@ -4215,9 +4735,15 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
+      <c r="B37" s="7">
+        <v>42946</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="4">
+        <v>27</v>
+      </c>
       <c r="E37" s="5"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -4231,9 +4757,15 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
+      <c r="B38" s="6">
+        <v>42947</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2">
+        <v>27</v>
+      </c>
       <c r="E38" s="3"/>
       <c r="F38" s="8"/>
       <c r="G38" s="2"/>
@@ -4247,9 +4779,15 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
+      <c r="B39" s="7">
+        <v>42948</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="4">
+        <v>27</v>
+      </c>
       <c r="E39" s="5"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -4263,9 +4801,15 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="3"/>
+      <c r="B40" s="6">
+        <v>42949</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <v>27</v>
+      </c>
       <c r="E40" s="5"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -4279,9 +4823,15 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="5"/>
+      <c r="B41" s="7">
+        <v>42950</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="4">
+        <v>27</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="8"/>
       <c r="G41" s="2"/>
@@ -4295,9 +4845,15 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="3"/>
+      <c r="B42" s="6">
+        <v>42951</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2">
+        <v>27</v>
+      </c>
       <c r="E42" s="5"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -4311,9 +4867,15 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="5"/>
+      <c r="B43" s="7">
+        <v>42952</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="4">
+        <v>27</v>
+      </c>
       <c r="E43" s="3"/>
       <c r="F43" s="8"/>
       <c r="G43" s="2"/>
@@ -4327,9 +4889,15 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="3"/>
+      <c r="B44" s="6">
+        <v>42953</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="2">
+        <v>27</v>
+      </c>
       <c r="E44" s="5"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -4343,9 +4911,15 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="5"/>
+      <c r="B45" s="7">
+        <v>42954</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="4">
+        <v>27</v>
+      </c>
       <c r="E45" s="3"/>
       <c r="F45" s="8"/>
       <c r="G45" s="2"/>
@@ -4359,9 +4933,15 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="3"/>
+      <c r="B46" s="6">
+        <v>42955</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="2">
+        <v>27</v>
+      </c>
       <c r="E46" s="5"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -4375,9 +4955,15 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="5"/>
+      <c r="B47" s="7">
+        <v>42956</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4">
+        <v>27</v>
+      </c>
       <c r="E47" s="3"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -4390,249 +4976,379 @@
       <c r="N47" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B24:B31 A26 C26 G26 I32:J32 L32 I38:J38 L38 I41:J41 L41 I47:J47 L47 E26 A24:C25 A27:C27 A29:C29 A31:C32 A37:C38 A40:C41 A46:C47 A3:F3 A7:F7 A11:F11 A19:F19 A23:F23 A4:E4 A8:E8 A12:E12 A15:D16 A20:E20 E47 E41 E38 E32 E46:F46 E40:F40 E37:F37 E31:F31 E29:H29 E27:H27 E24:L25">
-    <cfRule type="timePeriod" dxfId="48" priority="51" timePeriod="today">
+  <conditionalFormatting sqref="I32:J32 L32 I38:J38 L38 I41:J41 L41 I47:J47 L47 A24:A27 A29 A37:A38 A40:A41 A46:A47 A3:F3 A7:F7 A11:F11 A19:F19 A23:D23 A4:E4 A8:E8 A12:E12 A15:D16 A20:D20 E41 E38 E32 E46:F46 E40:F40 E37:F37 E31:F31 H29 H27 H24:L25 B24:D24 B27:C28 A31:D32 B35:D36 B39:D40 B43:D44 B47:E47">
+    <cfRule type="timePeriod" dxfId="77" priority="81" timePeriod="today">
       <formula>FLOOR(A3,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26:L31 H26 F26 A28:C28 A30:C30 F28:H28 F30:H30 H31 I33:L36 H37:L37 I39:L39 H40:L40 I42:L45 H46:L46">
-    <cfRule type="timePeriod" dxfId="47" priority="50" timePeriod="today">
+  <conditionalFormatting sqref="I26:L31 H26 A28 A30 H28 H30:H31 I33:L36 H37:L37 I39:L39 H40:L40 I42:L45 H46:L46">
+    <cfRule type="timePeriod" dxfId="76" priority="80" timePeriod="today">
       <formula>FLOOR(A26,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:B36 B38:B39 B41:B45 B47">
-    <cfRule type="timePeriod" dxfId="46" priority="49" timePeriod="today">
-      <formula>FLOOR(B32,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33:C36 H32:H36 A39:C39 H38:H39 A42:C45 H41:H45 H47">
-    <cfRule type="timePeriod" dxfId="45" priority="48" timePeriod="today">
+  <conditionalFormatting sqref="H32:H36 A39 H38:H39 A42:A45 H41:H45 H47 A33:A36">
+    <cfRule type="timePeriod" dxfId="75" priority="78" timePeriod="today">
       <formula>FLOOR(A32,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F32 F38 F41 F47">
+    <cfRule type="timePeriod" dxfId="74" priority="74" timePeriod="today">
+      <formula>FLOOR(F32,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31:G32 G37:G38 G40:G41 G46:G47">
+    <cfRule type="timePeriod" dxfId="73" priority="73" timePeriod="today">
+      <formula>FLOOR(G31,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32 K38 K41 K47">
+    <cfRule type="timePeriod" dxfId="72" priority="72" timePeriod="today">
+      <formula>FLOOR(K32,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33:F33 E39:F39 E42:F42">
+    <cfRule type="timePeriod" dxfId="71" priority="70" timePeriod="today">
+      <formula>FLOOR(E33,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34 E43">
+    <cfRule type="timePeriod" dxfId="70" priority="69" timePeriod="today">
+      <formula>FLOOR(E34,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F34 F43">
+    <cfRule type="timePeriod" dxfId="69" priority="68" timePeriod="today">
+      <formula>FLOOR(F34,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33:G34 G39 G42:G43">
+    <cfRule type="timePeriod" dxfId="68" priority="67" timePeriod="today">
+      <formula>FLOOR(G33,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35:F35 E44:F44">
+    <cfRule type="timePeriod" dxfId="67" priority="66" timePeriod="today">
+      <formula>FLOOR(E35,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36 E45">
+    <cfRule type="timePeriod" dxfId="66" priority="65" timePeriod="today">
+      <formula>FLOOR(E36,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36 F45">
+    <cfRule type="timePeriod" dxfId="65" priority="64" timePeriod="today">
+      <formula>FLOOR(F36,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35:G36 G44:G45">
+    <cfRule type="timePeriod" dxfId="64" priority="63" timePeriod="today">
+      <formula>FLOOR(G35,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3 I4:J4 L4 B7 B11 B15 B19 B23 I8:J8 I12:J12 I16:J16 I20:J20 L8 L12 L16 L20 B27 B31 B35 B39 B43 B47">
+    <cfRule type="timePeriod" dxfId="63" priority="62" timePeriod="today">
+      <formula>FLOOR(B3,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:L2 H3:L3 I5:L6 H7:L7 H11:L11 H15:L15 H19:L19 H23:L23 I9:L10 I13:L14 I17:L18 I21:L22">
+    <cfRule type="timePeriod" dxfId="62" priority="61" timePeriod="today">
+      <formula>FLOOR(H2,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2 B4:B6 B8:B10 B12:B14 B16:B18 B20:B22 B24:B26 B28:B30 B32:B34 B36:B38 B40:B42 B44:B46">
+    <cfRule type="timePeriod" dxfId="61" priority="60" timePeriod="today">
+      <formula>FLOOR(B2,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:D2 H2 A5:D6 H4:H6 A9:D10 A13:D14 A17:D18 A21:D22 H8:H10 H12:H14 H16:H18 H20:H22 B25:D26 B29:C30 B33:D34 B37:D38 B41:D42 B45:D46 D2:D26 D31:D47">
+    <cfRule type="timePeriod" dxfId="60" priority="59" timePeriod="today">
+      <formula>FLOOR(A2,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4 F8">
+    <cfRule type="timePeriod" dxfId="59" priority="58" timePeriod="today">
+      <formula>FLOOR(F4,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G4 G7:G8 G11 G19">
+    <cfRule type="timePeriod" dxfId="58" priority="57" timePeriod="today">
+      <formula>FLOOR(G3,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4 K8 K12 K16 K20">
+    <cfRule type="timePeriod" dxfId="57" priority="56" timePeriod="today">
+      <formula>FLOOR(K4,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:F5 E9:F9 E13">
+    <cfRule type="timePeriod" dxfId="56" priority="55" timePeriod="today">
+      <formula>FLOOR(E5,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5 G9 G13">
+    <cfRule type="timePeriod" dxfId="55" priority="54" timePeriod="today">
+      <formula>FLOOR(G5,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2 E6 E10 E14">
+    <cfRule type="timePeriod" dxfId="54" priority="53" timePeriod="today">
+      <formula>FLOOR(E2,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2 F6">
+    <cfRule type="timePeriod" dxfId="53" priority="52" timePeriod="today">
+      <formula>FLOOR(F2,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2 G6 G10 G14">
+    <cfRule type="timePeriod" dxfId="52" priority="51" timePeriod="today">
+      <formula>FLOOR(G2,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="timePeriod" dxfId="51" priority="50" timePeriod="today">
+      <formula>FLOOR(F10,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M32 M38 M41 M47 M24:M25">
+    <cfRule type="timePeriod" dxfId="50" priority="49" timePeriod="today">
+      <formula>FLOOR(M24,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M26:M31 M33:M37 M39:M40 M42:M46">
+    <cfRule type="timePeriod" dxfId="49" priority="48" timePeriod="today">
+      <formula>FLOOR(M26,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4 M8 M12 M16 M20">
+    <cfRule type="timePeriod" dxfId="48" priority="47" timePeriod="today">
+      <formula>FLOOR(M4,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M3 M5:M7 M9:M11 M13:M15 M17:M19 M21:M23">
+    <cfRule type="timePeriod" dxfId="47" priority="46" timePeriod="today">
+      <formula>FLOOR(M2,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N32 N38 N41 N47 N24 N28">
+    <cfRule type="timePeriod" dxfId="46" priority="44" timePeriod="today">
+      <formula>FLOOR(N24,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N33:N37 N39:N40 N42:N46">
+    <cfRule type="timePeriod" dxfId="45" priority="43" timePeriod="today">
+      <formula>FLOOR(N33,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4 N8 N12 N16 N20">
+    <cfRule type="timePeriod" dxfId="44" priority="42" timePeriod="today">
+      <formula>FLOOR(N4,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N3 N5:N7 N9:N11 N13:N15 N17:N19 N21:N23 N25:N27 N29:N31">
+    <cfRule type="timePeriod" dxfId="43" priority="41" timePeriod="today">
+      <formula>FLOOR(N2,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="timePeriod" dxfId="42" priority="40" timePeriod="today">
+      <formula>FLOOR(G12,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="timePeriod" dxfId="41" priority="39" timePeriod="today">
+      <formula>FLOOR(F12,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="timePeriod" dxfId="40" priority="38" timePeriod="today">
+      <formula>FLOOR(F13,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="timePeriod" dxfId="39" priority="37" timePeriod="today">
+      <formula>FLOOR(F14,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15 E17">
+    <cfRule type="timePeriod" dxfId="38" priority="36" timePeriod="today">
+      <formula>FLOOR(E15,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15 G17">
+    <cfRule type="timePeriod" dxfId="37" priority="35" timePeriod="today">
+      <formula>FLOOR(G15,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16 E18">
+    <cfRule type="timePeriod" dxfId="36" priority="34" timePeriod="today">
+      <formula>FLOOR(E16,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16 G18">
+    <cfRule type="timePeriod" dxfId="35" priority="33" timePeriod="today">
+      <formula>FLOOR(G16,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15 F17">
+    <cfRule type="timePeriod" dxfId="34" priority="32" timePeriod="today">
+      <formula>FLOOR(F15,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16 F18">
+    <cfRule type="timePeriod" dxfId="33" priority="31" timePeriod="today">
+      <formula>FLOOR(F16,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="timePeriod" dxfId="32" priority="30" timePeriod="today">
+      <formula>FLOOR(E20,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20">
+    <cfRule type="timePeriod" dxfId="31" priority="29" timePeriod="today">
+      <formula>FLOOR(G20,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="timePeriod" dxfId="30" priority="28" timePeriod="today">
+      <formula>FLOOR(F20,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21:F21">
+    <cfRule type="timePeriod" dxfId="29" priority="27" timePeriod="today">
+      <formula>FLOOR(E21,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21">
+    <cfRule type="timePeriod" dxfId="28" priority="26" timePeriod="today">
+      <formula>FLOOR(G21,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="timePeriod" dxfId="27" priority="25" timePeriod="today">
+      <formula>FLOOR(E22,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22">
+    <cfRule type="timePeriod" dxfId="26" priority="24" timePeriod="today">
+      <formula>FLOOR(G22,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="timePeriod" dxfId="25" priority="23" timePeriod="today">
+      <formula>FLOOR(F22,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:F23">
+    <cfRule type="timePeriod" dxfId="24" priority="22" timePeriod="today">
+      <formula>FLOOR(E23,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="timePeriod" dxfId="23" priority="21" timePeriod="today">
+      <formula>FLOOR(G23,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="timePeriod" dxfId="22" priority="20" timePeriod="today">
+      <formula>FLOOR(E24,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="timePeriod" dxfId="21" priority="19" timePeriod="today">
+      <formula>FLOOR(G24,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="timePeriod" dxfId="20" priority="18" timePeriod="today">
+      <formula>FLOOR(F24,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:F25">
+    <cfRule type="timePeriod" dxfId="19" priority="17" timePeriod="today">
+      <formula>FLOOR(E25,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25">
+    <cfRule type="timePeriod" dxfId="18" priority="16" timePeriod="today">
+      <formula>FLOOR(G25,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="timePeriod" dxfId="17" priority="15" timePeriod="today">
+      <formula>FLOOR(E26,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26">
+    <cfRule type="timePeriod" dxfId="16" priority="14" timePeriod="today">
+      <formula>FLOOR(G26,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="timePeriod" dxfId="15" priority="13" timePeriod="today">
+      <formula>FLOOR(F26,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:D28">
+    <cfRule type="timePeriod" dxfId="14" priority="12" timePeriod="today">
+      <formula>FLOOR(D27,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27:F27">
+    <cfRule type="timePeriod" dxfId="13" priority="11" timePeriod="today">
+      <formula>FLOOR(E27,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27">
+    <cfRule type="timePeriod" dxfId="12" priority="10" timePeriod="today">
+      <formula>FLOOR(G27,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="timePeriod" dxfId="44" priority="46" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="11" priority="9" timePeriod="today">
       <formula>FLOOR(E28,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="timePeriod" dxfId="10" priority="8" timePeriod="today">
+      <formula>FLOOR(G28,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
+    <cfRule type="timePeriod" dxfId="9" priority="7" timePeriod="today">
+      <formula>FLOOR(F28,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:D30">
+    <cfRule type="timePeriod" dxfId="8" priority="6" timePeriod="today">
+      <formula>FLOOR(D29,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29:F29">
+    <cfRule type="timePeriod" dxfId="7" priority="5" timePeriod="today">
+      <formula>FLOOR(E29,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29">
+    <cfRule type="timePeriod" dxfId="6" priority="4" timePeriod="today">
+      <formula>FLOOR(G29,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="timePeriod" dxfId="43" priority="45" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="5" priority="3" timePeriod="today">
       <formula>FLOOR(E30,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F32 F38 F41 F47">
-    <cfRule type="timePeriod" dxfId="42" priority="44" timePeriod="today">
-      <formula>FLOOR(F32,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31:G32 G37:G38 G40:G41 G46:G47">
-    <cfRule type="timePeriod" dxfId="41" priority="43" timePeriod="today">
-      <formula>FLOOR(G31,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32 K38 K41 K47">
-    <cfRule type="timePeriod" dxfId="40" priority="42" timePeriod="today">
-      <formula>FLOOR(K32,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33:F33 E39:F39 E42:F42">
-    <cfRule type="timePeriod" dxfId="39" priority="40" timePeriod="today">
-      <formula>FLOOR(E33,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34 E43">
-    <cfRule type="timePeriod" dxfId="38" priority="39" timePeriod="today">
-      <formula>FLOOR(E34,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F34 F43">
-    <cfRule type="timePeriod" dxfId="37" priority="38" timePeriod="today">
-      <formula>FLOOR(F34,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33:G34 G39 G42:G43">
-    <cfRule type="timePeriod" dxfId="36" priority="37" timePeriod="today">
-      <formula>FLOOR(G33,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35:F35 E44:F44">
-    <cfRule type="timePeriod" dxfId="35" priority="36" timePeriod="today">
-      <formula>FLOOR(E35,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36 E45">
-    <cfRule type="timePeriod" dxfId="34" priority="35" timePeriod="today">
-      <formula>FLOOR(E36,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F36 F45">
-    <cfRule type="timePeriod" dxfId="33" priority="34" timePeriod="today">
-      <formula>FLOOR(F36,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35:G36 G44:G45">
-    <cfRule type="timePeriod" dxfId="32" priority="33" timePeriod="today">
-      <formula>FLOOR(G35,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3 I4:J4 L4 B7 B11 B15 B19 B23 I8:J8 I12:J12 I16:J16 I20:J20 L8 L12 L16 L20">
-    <cfRule type="timePeriod" dxfId="31" priority="32" timePeriod="today">
-      <formula>FLOOR(B3,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:L2 H3:L3 I5:L6 H7:L7 H11:L11 H15:L15 H19:L19 H23:L23 I9:L10 I13:L14 I17:L18 I21:L22">
-    <cfRule type="timePeriod" dxfId="30" priority="31" timePeriod="today">
-      <formula>FLOOR(H2,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2 B4:B6 B8:B10 B12:B14 B16:B18 B20:B22">
-    <cfRule type="timePeriod" dxfId="29" priority="30" timePeriod="today">
-      <formula>FLOOR(B2,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:D2 H2 A5:D6 H4:H6 A9:D10 A13:D14 A17:D18 A21:D22 H8:H10 H12:H14 H16:H18 H20:H22 D2:D23">
-    <cfRule type="timePeriod" dxfId="28" priority="29" timePeriod="today">
-      <formula>FLOOR(A2,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4 F8 F20">
-    <cfRule type="timePeriod" dxfId="27" priority="28" timePeriod="today">
-      <formula>FLOOR(F4,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G4 G7:G8 G11 G19:G20 G23">
-    <cfRule type="timePeriod" dxfId="26" priority="27" timePeriod="today">
-      <formula>FLOOR(G3,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4 K8 K12 K16 K20">
-    <cfRule type="timePeriod" dxfId="25" priority="26" timePeriod="today">
-      <formula>FLOOR(K4,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:F5 E9:F9 E13 E21:F21">
-    <cfRule type="timePeriod" dxfId="24" priority="25" timePeriod="today">
-      <formula>FLOOR(E5,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5 G9 G13 G21">
-    <cfRule type="timePeriod" dxfId="23" priority="24" timePeriod="today">
-      <formula>FLOOR(G5,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2 E6 E10 E14 E22">
-    <cfRule type="timePeriod" dxfId="22" priority="23" timePeriod="today">
-      <formula>FLOOR(E2,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2 F6 F22">
-    <cfRule type="timePeriod" dxfId="21" priority="22" timePeriod="today">
-      <formula>FLOOR(F2,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2 G6 G10 G14 G22">
-    <cfRule type="timePeriod" dxfId="20" priority="21" timePeriod="today">
-      <formula>FLOOR(G2,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="timePeriod" dxfId="19" priority="20" timePeriod="today">
-      <formula>FLOOR(F10,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M32 M38 M41 M47 M24:M25">
-    <cfRule type="timePeriod" dxfId="18" priority="19" timePeriod="today">
-      <formula>FLOOR(M24,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M26:M31 M33:M37 M39:M40 M42:M46">
-    <cfRule type="timePeriod" dxfId="17" priority="18" timePeriod="today">
-      <formula>FLOOR(M26,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M4 M8 M12 M16 M20">
-    <cfRule type="timePeriod" dxfId="16" priority="17" timePeriod="today">
-      <formula>FLOOR(M4,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M3 M5:M7 M9:M11 M13:M15 M17:M19 M21:M23">
-    <cfRule type="timePeriod" dxfId="15" priority="16" timePeriod="today">
-      <formula>FLOOR(M2,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D47">
-    <cfRule type="timePeriod" dxfId="14" priority="15" timePeriod="today">
-      <formula>FLOOR(D24,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N32 N38 N41 N47 N24:N25">
-    <cfRule type="timePeriod" dxfId="13" priority="14" timePeriod="today">
-      <formula>FLOOR(N24,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N26:N31 N33:N37 N39:N40 N42:N46">
-    <cfRule type="timePeriod" dxfId="12" priority="13" timePeriod="today">
-      <formula>FLOOR(N26,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N4 N8 N12 N16 N20">
-    <cfRule type="timePeriod" dxfId="11" priority="12" timePeriod="today">
-      <formula>FLOOR(N4,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N3 N5:N7 N9:N11 N13:N15 N17:N19 N21:N23">
-    <cfRule type="timePeriod" dxfId="10" priority="11" timePeriod="today">
-      <formula>FLOOR(N2,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
-    <cfRule type="timePeriod" dxfId="9" priority="10" timePeriod="today">
-      <formula>FLOOR(G12,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="timePeriod" dxfId="8" priority="9" timePeriod="today">
-      <formula>FLOOR(F12,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
-    <cfRule type="timePeriod" dxfId="7" priority="8" timePeriod="today">
-      <formula>FLOOR(F13,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F14">
-    <cfRule type="timePeriod" dxfId="6" priority="7" timePeriod="today">
-      <formula>FLOOR(F14,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15 E17">
-    <cfRule type="timePeriod" dxfId="5" priority="6" timePeriod="today">
-      <formula>FLOOR(E15,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G15 G17">
-    <cfRule type="timePeriod" dxfId="4" priority="5" timePeriod="today">
-      <formula>FLOOR(G15,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16 E18">
-    <cfRule type="timePeriod" dxfId="3" priority="4" timePeriod="today">
-      <formula>FLOOR(E16,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G16 G18">
-    <cfRule type="timePeriod" dxfId="2" priority="3" timePeriod="today">
-      <formula>FLOOR(G16,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15 F17">
-    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="today">
-      <formula>FLOOR(F15,1)=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F16 F18">
-    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="today">
-      <formula>FLOOR(F16,1)=TODAY()</formula>
+  <conditionalFormatting sqref="G30">
+    <cfRule type="timePeriod" dxfId="4" priority="2" timePeriod="today">
+      <formula>FLOOR(G30,1)=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30">
+    <cfRule type="timePeriod" dxfId="3" priority="1" timePeriod="today">
+      <formula>FLOOR(F30,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>